<commit_message>
adding support for ranges on numeric-value fields; cleaning up the spreadsheets
</commit_message>
<xml_diff>
--- a/DnaRepairSpreadsheetParser/test/exampleData/broadAssays/Broad Institute- Jimmy Theriault V5.xlsx
+++ b/DnaRepairSpreadsheetParser/test/exampleData/broadAssays/Broad Institute- Jimmy Theriault V5.xlsx
@@ -4271,7 +4271,9 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:BH7600"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="F103" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G6" sqref="G6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
@@ -4934,18 +4936,18 @@
       <c r="A6" t="s">
         <v>90</v>
       </c>
-      <c r="G6" t="s">
-        <v>368</v>
-      </c>
-      <c r="H6" s="4" t="s">
-        <v>1136</v>
-      </c>
       <c r="I6" s="4"/>
       <c r="J6">
         <v>100</v>
       </c>
       <c r="K6" t="s">
         <v>303</v>
+      </c>
+      <c r="N6" s="4" t="s">
+        <v>1136</v>
+      </c>
+      <c r="O6" t="s">
+        <v>368</v>
       </c>
       <c r="AJ6" t="s">
         <v>91</v>
@@ -66983,13 +66985,13 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H198 H3:H5 H220:H221 H217:H218 H214:H215 H207:H212 H178 H180 H174:H176 H184 H38:H41 H156:H161 H153:H154 H148:H151 H145 H135:H143 H131:H133 H124:H129 H7:H10 H12:H13 H15:H18 H21:H26 H28:H30 H32 H36 H43:H48 H50:H52 H54:H56 H58:H59 H61 H65:H67 H69:H71 H73:H74 H85:H88 H76:H79 H81:H83 H90:H91 H93:H95 H97:H98 H100:H102 H106 H110:H112 H114:H117 H119:H122 H163:H164 H166 H168 H170 H172 H182 H194 H192 H188 H186 H190 H196 H200 H202:H205">
       <formula1>assay_component_type</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H123 I3:I124 H222 I216:I222 H219 I213:I214 I208:I211 I206 I148:I165 H37 H6 I142:I144 I140 I126:I138 H134 H130 H11 H14 H19:H20 H27 H31 H33:H35 H49 H53 H57 H60 H62:H64 H68 H72 H75 H84 H89 H92 H96 H99 H103:H105 H107:H109 H113 H118 I202:I204 I175">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H123 I3:I124 H222 I216:I222 H219 I213:I214 I208:I211 I206 I148:I165 H37 N6 I142:I144 I140 I126:I138 H134 H130 H11 H14 H19:H20 H27 H31 H33:H35 H49 H53 H57 H60 H62:H64 H68 H72 H75 H84 H89 H92 H96 H99 H103:H105 H107:H109 H113 H118 I202:I204 I175">
       <formula1>cultured_cell_name</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B74:B77 C3:C222 B98:B101">
       <formula1>biology</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H42 G3:G222 H155 H152 H162 H165 H80">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H42 H155 H152 H162 H165 H80 O6 G3:G5 G7:G222">
       <formula1>assay_component_role</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L182 K3:K222 L192 L194 L184 L188 L196 L198 L186">
@@ -67010,7 +67012,7 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M3:M222">
       <formula1>species_name</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="O3:O222">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="O3:O5 O7:O222">
       <formula1>detection_role</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="P3:P222">

</xml_diff>